<commit_message>
Adiciona teste com valores preenchidos a planilha de teste
</commit_message>
<xml_diff>
--- a/selenium-lab-main/Mapeamento de testes - Avaliação 2.xlsx
+++ b/selenium-lab-main/Mapeamento de testes - Avaliação 2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
   <si>
     <t>Caso de teste</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>Quantidade e data vazios e código, nome e valor preenchidos</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>Produto é cadastrado e modal é fechado</t>
   </si>
   <si>
     <t>1. Equipe de desenvolvimento deve proibir o cadastro de produtos com código iguais;</t>
@@ -273,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -299,9 +305,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -961,10 +964,10 @@
       <c r="B10" s="2">
         <v>8.0</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="2">
         <v>1.0</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>48</v>
       </c>
       <c r="E10" s="2">
@@ -1005,31 +1008,48 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="s">
+      <c r="A12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>100.0</v>
+      </c>
+      <c r="G12" s="9">
+        <v>45625.0</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1041,7 +1061,7 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1051,11 +1071,23 @@
       <c r="G16" s="5"/>
       <c r="H16" s="6"/>
     </row>
+    <row r="17">
+      <c r="A17" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A14:H14"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A17:H17"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualiza testes da planilha
</commit_message>
<xml_diff>
--- a/selenium-lab-main/Mapeamento de testes - Avaliação 2.xlsx
+++ b/selenium-lab-main/Mapeamento de testes - Avaliação 2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
   <si>
     <t>Caso de teste</t>
   </si>
@@ -173,7 +173,52 @@
     <t>Produto é cadastrado e aparece na página de produtos</t>
   </si>
   <si>
-    <t>1. Equipe de desenvolvimento deve proibir o cadastro de produtos com código iguais;</t>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deve abrir o modal de cadastro de produto ao clicar no botão de criar </t>
+  </si>
+  <si>
+    <t>Falha</t>
+  </si>
+  <si>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deve abrir o modal de cadastro de produto ao clicar no botão de editar </t>
+  </si>
+  <si>
+    <t>TC013</t>
+  </si>
+  <si>
+    <t>Deve excluir o produto ao clicar no botão de excluir</t>
+  </si>
+  <si>
+    <t>TC014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deve voltar para a página de login ao clicar no botão de voltar </t>
+  </si>
+  <si>
+    <t>TC015</t>
+  </si>
+  <si>
+    <t>Deve emitir uma mensagem de erro ao tentar cadastrar um produto com mesmo código de um já existente</t>
+  </si>
+  <si>
+    <t>TC016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deve fechar o modal ao clicar no botão de sair </t>
+  </si>
+  <si>
+    <t>Sucesso</t>
+  </si>
+  <si>
+    <t>1. Equipe de desenvolvimento deve padronizar a lingua da página;</t>
   </si>
   <si>
     <t>2. Equipe de desenvolvimento deve proibir o cadastro com valores negativos;</t>
@@ -987,7 +1032,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="2">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="C11" s="2">
         <v>1.0</v>
@@ -1012,7 +1057,7 @@
         <v>51</v>
       </c>
       <c r="B12" s="2">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="C12" s="2">
         <v>1.0</v>
@@ -1037,57 +1082,231 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="A13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="2">
+        <v>14.0</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="2">
+        <v>16.0</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A23:H23"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adiciona mais testes à classe de produtoTest
</commit_message>
<xml_diff>
--- a/selenium-lab-main/Mapeamento de testes - Avaliação 2.xlsx
+++ b/selenium-lab-main/Mapeamento de testes - Avaliação 2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="73">
   <si>
     <t>Caso de teste</t>
   </si>
@@ -131,6 +131,18 @@
     <t>Data</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deve voltar para a página de login ao clicar no botão de voltar </t>
+  </si>
+  <si>
+    <t>Falha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deve abrir o modal de cadastro de produto ao clicar no botão de criar </t>
+  </si>
+  <si>
     <t>Código, nome, quantidade, valor e data vazios</t>
   </si>
   <si>
@@ -158,64 +170,61 @@
     <t>Quantidade, valor e data vazios e código e nome preenchidos</t>
   </si>
   <si>
+    <t>TC010</t>
+  </si>
+  <si>
     <t>Relógio de pulso</t>
   </si>
   <si>
     <t>Valor e data vazios e código, nome e quantidade preenchidos</t>
   </si>
   <si>
+    <t>TC011</t>
+  </si>
+  <si>
     <t>Quantidade e data vazios e código, nome e valor preenchidos</t>
   </si>
   <si>
-    <t>TC010</t>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t>Código, nome, quantidade, valor e data preenchidos</t>
   </si>
   <si>
     <t>Produto é cadastrado e aparece na página de produtos</t>
   </si>
   <si>
-    <t>TC011</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deve abrir o modal de cadastro de produto ao clicar no botão de criar </t>
-  </si>
-  <si>
-    <t>Falha</t>
-  </si>
-  <si>
-    <t>TC012</t>
+    <t>TC013</t>
+  </si>
+  <si>
+    <t>Deve emitir uma mensagem de erro ao tentar cadastrar um produto com mesmo código de um já existente</t>
+  </si>
+  <si>
+    <t>TC014</t>
+  </si>
+  <si>
+    <t>Deve fechar o modal ao clicar no botão de sair sem ter cadastrado nenhum produto</t>
+  </si>
+  <si>
+    <t>TC015</t>
+  </si>
+  <si>
+    <t>Deve fechar o modal ao clicar no botão de sair ao cadastrar um produto</t>
+  </si>
+  <si>
+    <t>Sucesso</t>
+  </si>
+  <si>
+    <t>TC016</t>
   </si>
   <si>
     <t xml:space="preserve">Deve abrir o modal de cadastro de produto ao clicar no botão de editar </t>
   </si>
   <si>
-    <t>TC013</t>
+    <t>TC017</t>
   </si>
   <si>
     <t>Deve excluir o produto ao clicar no botão de excluir</t>
-  </si>
-  <si>
-    <t>TC014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deve voltar para a página de login ao clicar no botão de voltar </t>
-  </si>
-  <si>
-    <t>TC015</t>
-  </si>
-  <si>
-    <t>Deve emitir uma mensagem de erro ao tentar cadastrar um produto com mesmo código de um já existente</t>
-  </si>
-  <si>
-    <t>TC016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deve fechar o modal ao clicar no botão de sair </t>
-  </si>
-  <si>
-    <t>Sucesso</t>
   </si>
   <si>
     <t>1. Equipe de desenvolvimento deve padronizar a lingua da página;</t>
@@ -862,37 +871,55 @@
       <c r="B3" s="2">
         <v>1.0</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="C3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="H3" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2">
         <v>2.0</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="9">
-        <v>45625.0</v>
+      <c r="C4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -902,39 +929,37 @@
       <c r="B5" s="2">
         <v>3.0</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="2">
-        <v>100.0</v>
-      </c>
+      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2">
         <v>4.0</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="9">
+        <v>45625.0</v>
+      </c>
       <c r="H6" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7">
@@ -944,39 +969,39 @@
       <c r="B7" s="2">
         <v>5.0</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2">
+        <v>100.0</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="2">
         <v>6.0</v>
       </c>
-      <c r="C8" s="2">
-        <v>1.0</v>
-      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <v>3.0</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9">
@@ -986,24 +1011,22 @@
       <c r="B9" s="2">
         <v>7.0</v>
       </c>
-      <c r="C9" s="2">
-        <v>1.0</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="2">
@@ -1012,19 +1035,15 @@
       <c r="C10" s="2">
         <v>1.0</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="2">
-        <v>3.0</v>
-      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11">
@@ -1041,20 +1060,18 @@
         <v>48</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2">
-        <v>100.0</v>
-      </c>
+      <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>51</v>
+      <c r="A12" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="B12" s="2">
         <v>10.0</v>
@@ -1062,52 +1079,44 @@
       <c r="C12" s="2">
         <v>1.0</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>48</v>
+      <c r="D12" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="E12" s="2">
         <v>3.0</v>
       </c>
-      <c r="F12" s="2">
-        <v>100.0</v>
-      </c>
-      <c r="G12" s="9">
-        <v>45625.0</v>
-      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B13" s="2">
         <v>11.0</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>54</v>
+      <c r="C13" s="2">
+        <v>1.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
+        <v>100.0</v>
+      </c>
+      <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14">
@@ -1117,170 +1126,187 @@
       <c r="B14" s="2">
         <v>12.0</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>54</v>
+      <c r="C14" s="2">
+        <v>1.0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>100.0</v>
+      </c>
+      <c r="G14" s="9">
+        <v>45625.0</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>58</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="s">
-        <v>59</v>
+      <c r="A15" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="B15" s="2">
         <v>13.0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B16" s="2">
         <v>14.0</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B17" s="2">
         <v>15.0</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="s">
-        <v>65</v>
+      <c r="A18" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="B18" s="2">
         <v>16.0</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="4" t="s">
+      <c r="A19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1292,7 +1318,7 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1302,11 +1328,23 @@
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
     </row>
+    <row r="24">
+      <c r="A24" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A24:H24"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>